<commit_message>
feat: update excel doctor schedule template
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/xlsx/template_doctor_schedule.xlsx
+++ b/src/main/resources/templates/xlsx/template_doctor_schedule.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t xml:space="preserve">Lịch Sử Khám Bệnh Tháng ${date}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ngày xuất: ${dateExport}</t>
+    <t xml:space="preserve">Lịch Sử Khám Bệnh ${date}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngày xuất: ${exportDate}</t>
   </si>
   <si>
     <t xml:space="preserve">Tên bác sĩ: ${doctorName}</t>
@@ -59,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -82,12 +82,6 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="20"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -95,19 +89,15 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -168,19 +158,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -189,10 +183,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -321,8 +311,8 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -332,15 +322,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="29.32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -352,7 +342,6 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="0"/>
       <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
@@ -363,41 +352,40 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="0"/>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="5"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="8" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
   </mergeCells>

</xml_diff>

<commit_message>
feat: update pdf export, working now
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/xlsx/template_doctor_schedule.xlsx
+++ b/src/main/resources/templates/xlsx/template_doctor_schedule.xlsx
@@ -59,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -85,12 +85,6 @@
       <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val=""/>
-      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -149,17 +143,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -170,15 +160,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -311,8 +293,8 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -338,48 +320,48 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="F2" s="4" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="F3" s="5" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="6"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>